<commit_message>
minors updates for release
</commit_message>
<xml_diff>
--- a/simfin/params/gr_A.xlsx
+++ b/simfin/params/gr_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliennavaux/Dropbox (CEDIA)/simfin/Model/simfin/params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DAEABB-EE55-704F-B003-1B927442650A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331F06EF-03E3-5441-AC68-E314E47C982E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17200" yWindow="4480" windowWidth="20920" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,13 +42,13 @@
     <t>0.005856088432586781</t>
   </si>
   <si>
-    <t>0.024778</t>
+    <t>0.0226</t>
   </si>
   <si>
-    <t>0.023265</t>
+    <t>0.00905</t>
   </si>
   <si>
-    <t>0.009555</t>
+    <t>0.023809</t>
   </si>
 </sst>
 </file>
@@ -1155,13 +1155,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>

</xml_diff>